<commit_message>
starting playoff. still need to fill out service tests
</commit_message>
<xml_diff>
--- a/docs/math_stuff.xlsx
+++ b/docs/math_stuff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\python_learning\team_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D199AB3-C081-42C2-8412-E5567C5E8867}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B869B-2BA4-4F1B-A20F-E41A4F00F49C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6910" activeTab="5" xr2:uid="{90D94824-A6D7-4CA6-B1FC-4C1AA4DBBDD0}"/>
   </bookViews>
@@ -24394,7 +24394,7 @@
   <dimension ref="A1:EE2002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="DH1" workbookViewId="0">
-      <selection activeCell="DX1" sqref="DX1:DX21"/>
+      <selection activeCell="EA1" sqref="EA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24494,8 +24494,8 @@
         <v>0</v>
       </c>
       <c r="ED1">
-        <f>EB1/$EB$23*100</f>
-        <v>7.054176072234764</v>
+        <f>EB1/$EB$14*100</f>
+        <v>2.781641168289291</v>
       </c>
       <c r="EE1">
         <f>EC1*ED1</f>
@@ -24652,29 +24652,29 @@
       </c>
       <c r="DX2" t="str">
         <f t="shared" ref="DX2:DX21" si="0">_xlfn.CONCAT("[",EC2,",",EA2,",",DZ2,"],")</f>
-        <v>[1,500,1250],</v>
+        <v>[1,500,1500],</v>
       </c>
       <c r="DZ2">
         <f>EA2+EB2</f>
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="EA2">
         <f>DZ1</f>
         <v>500</v>
       </c>
       <c r="EB2">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="EC2">
         <v>1</v>
       </c>
       <c r="ED2">
-        <f t="shared" ref="ED2:ED21" si="1">EB2/$EB$23*100</f>
-        <v>10.581264108352144</v>
+        <f t="shared" ref="ED2:ED11" si="1">EB2/$EB$14*100</f>
+        <v>5.563282336578582</v>
       </c>
       <c r="EE2">
         <f t="shared" ref="EE2:EE21" si="2">EC2*ED2</f>
-        <v>10.581264108352144</v>
+        <v>5.563282336578582</v>
       </c>
     </row>
     <row r="3" spans="1:135" x14ac:dyDescent="0.35">
@@ -24967,29 +24967,29 @@
       </c>
       <c r="DX3" t="str">
         <f t="shared" si="0"/>
-        <v>[2,1250,2250],</v>
+        <v>[2,1500,4000],</v>
       </c>
       <c r="DZ3">
         <f t="shared" ref="DZ3:DZ21" si="3">EA3+EB3</f>
-        <v>2250</v>
+        <v>4000</v>
       </c>
       <c r="EA3">
         <f t="shared" ref="EA3:EA21" si="4">DZ2</f>
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="EB3">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="EC3">
         <v>2</v>
       </c>
       <c r="ED3">
         <f t="shared" si="1"/>
-        <v>14.108352144469528</v>
+        <v>13.908205841446453</v>
       </c>
       <c r="EE3">
         <f t="shared" si="2"/>
-        <v>28.216704288939056</v>
+        <v>27.816411682892905</v>
       </c>
     </row>
     <row r="4" spans="1:135" x14ac:dyDescent="0.35">
@@ -25351,29 +25351,29 @@
       </c>
       <c r="DX4" t="str">
         <f t="shared" si="0"/>
-        <v>[3,2250,3250],</v>
+        <v>[3,4000,9000],</v>
       </c>
       <c r="DZ4">
         <f t="shared" si="3"/>
-        <v>3250</v>
+        <v>9000</v>
       </c>
       <c r="EA4">
         <f t="shared" si="4"/>
-        <v>2250</v>
+        <v>4000</v>
       </c>
       <c r="EB4">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="EC4">
         <v>3</v>
       </c>
       <c r="ED4">
         <f t="shared" si="1"/>
-        <v>14.108352144469528</v>
+        <v>27.816411682892905</v>
       </c>
       <c r="EE4">
         <f t="shared" si="2"/>
-        <v>42.325056433408584</v>
+        <v>83.449235048678716</v>
       </c>
     </row>
     <row r="5" spans="1:135" x14ac:dyDescent="0.35">
@@ -25781,29 +25781,29 @@
       </c>
       <c r="DX5" t="str">
         <f t="shared" si="0"/>
-        <v>[4,3250,4250],</v>
+        <v>[4,9000,14000],</v>
       </c>
       <c r="DZ5">
         <f t="shared" si="3"/>
-        <v>4250</v>
+        <v>14000</v>
       </c>
       <c r="EA5">
         <f t="shared" si="4"/>
-        <v>3250</v>
+        <v>9000</v>
       </c>
       <c r="EB5">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="EC5">
         <v>4</v>
       </c>
       <c r="ED5">
         <f t="shared" si="1"/>
-        <v>14.108352144469528</v>
+        <v>27.816411682892905</v>
       </c>
       <c r="EE5">
         <f t="shared" si="2"/>
-        <v>56.433408577878112</v>
+        <v>111.26564673157162</v>
       </c>
     </row>
     <row r="6" spans="1:135" x14ac:dyDescent="0.35">
@@ -26234,29 +26234,29 @@
       </c>
       <c r="DX6" t="str">
         <f t="shared" si="0"/>
-        <v>[5,4250,5250],</v>
+        <v>[5,14000,16500],</v>
       </c>
       <c r="DZ6">
         <f t="shared" si="3"/>
-        <v>5250</v>
+        <v>16500</v>
       </c>
       <c r="EA6">
         <f t="shared" si="4"/>
-        <v>4250</v>
+        <v>14000</v>
       </c>
       <c r="EB6">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="EC6">
         <v>5</v>
       </c>
       <c r="ED6">
         <f t="shared" si="1"/>
-        <v>14.108352144469528</v>
+        <v>13.908205841446453</v>
       </c>
       <c r="EE6">
         <f t="shared" si="2"/>
-        <v>70.541760722347647</v>
+        <v>69.54102920723227</v>
       </c>
     </row>
     <row r="7" spans="1:135" x14ac:dyDescent="0.35">
@@ -26687,29 +26687,29 @@
       </c>
       <c r="DX7" t="str">
         <f t="shared" si="0"/>
-        <v>[6,5250,6000],</v>
+        <v>[6,16500,17500],</v>
       </c>
       <c r="DZ7">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>17500</v>
       </c>
       <c r="EA7">
         <f t="shared" si="4"/>
-        <v>5250</v>
+        <v>16500</v>
       </c>
       <c r="EB7">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="EC7">
         <v>6</v>
       </c>
       <c r="ED7">
         <f t="shared" si="1"/>
-        <v>10.581264108352144</v>
+        <v>5.563282336578582</v>
       </c>
       <c r="EE7">
         <f t="shared" si="2"/>
-        <v>63.487584650112865</v>
+        <v>33.379694019471494</v>
       </c>
     </row>
     <row r="8" spans="1:135" x14ac:dyDescent="0.35">
@@ -27140,29 +27140,29 @@
       </c>
       <c r="DX8" t="str">
         <f t="shared" si="0"/>
-        <v>[7,6000,6500],</v>
+        <v>[7,17500,17750],</v>
       </c>
       <c r="DZ8">
         <f t="shared" si="3"/>
-        <v>6500</v>
+        <v>17750</v>
       </c>
       <c r="EA8">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>17500</v>
       </c>
       <c r="EB8">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="EC8">
         <v>7</v>
       </c>
       <c r="ED8">
         <f t="shared" si="1"/>
-        <v>7.054176072234764</v>
+        <v>1.3908205841446455</v>
       </c>
       <c r="EE8">
         <f t="shared" si="2"/>
-        <v>49.379232505643344</v>
+        <v>9.7357440890125186</v>
       </c>
     </row>
     <row r="9" spans="1:135" x14ac:dyDescent="0.35">
@@ -27593,29 +27593,29 @@
       </c>
       <c r="DX9" t="str">
         <f t="shared" si="0"/>
-        <v>[8,6500,6750],</v>
+        <v>[8,17750,17875],</v>
       </c>
       <c r="DZ9">
         <f t="shared" si="3"/>
-        <v>6750</v>
+        <v>17875</v>
       </c>
       <c r="EA9">
         <f t="shared" si="4"/>
-        <v>6500</v>
+        <v>17750</v>
       </c>
       <c r="EB9">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="EC9">
         <v>8</v>
       </c>
       <c r="ED9">
         <f t="shared" si="1"/>
-        <v>3.527088036117382</v>
+        <v>0.69541029207232274</v>
       </c>
       <c r="EE9">
         <f t="shared" si="2"/>
-        <v>28.216704288939056</v>
+        <v>5.563282336578582</v>
       </c>
     </row>
     <row r="10" spans="1:135" x14ac:dyDescent="0.35">
@@ -28046,29 +28046,29 @@
       </c>
       <c r="DX10" t="str">
         <f t="shared" si="0"/>
-        <v>[9,6750,6875],</v>
+        <v>[9,17875,17950],</v>
       </c>
       <c r="DZ10">
         <f t="shared" si="3"/>
-        <v>6875</v>
+        <v>17950</v>
       </c>
       <c r="EA10">
         <f t="shared" si="4"/>
-        <v>6750</v>
+        <v>17875</v>
       </c>
       <c r="EB10">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="EC10">
         <v>9</v>
       </c>
       <c r="ED10">
         <f t="shared" si="1"/>
-        <v>1.763544018058691</v>
+        <v>0.41724617524339358</v>
       </c>
       <c r="EE10">
         <f t="shared" si="2"/>
-        <v>15.87189616252822</v>
+        <v>3.7552155771905422</v>
       </c>
     </row>
     <row r="11" spans="1:135" x14ac:dyDescent="0.35">
@@ -28499,29 +28499,29 @@
       </c>
       <c r="DX11" t="str">
         <f t="shared" si="0"/>
-        <v>[10,6875,6950],</v>
+        <v>[10,17950,17975],</v>
       </c>
       <c r="DZ11">
         <f t="shared" si="3"/>
-        <v>6950</v>
+        <v>17975</v>
       </c>
       <c r="EA11">
         <f t="shared" si="4"/>
-        <v>6875</v>
+        <v>17950</v>
       </c>
       <c r="EB11">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="EC11">
         <v>10</v>
       </c>
       <c r="ED11">
         <f t="shared" si="1"/>
-        <v>1.0581264108352144</v>
+        <v>0.13908205841446453</v>
       </c>
       <c r="EE11">
         <f t="shared" si="2"/>
-        <v>10.581264108352144</v>
+        <v>1.3908205841446453</v>
       </c>
     </row>
     <row r="12" spans="1:135" x14ac:dyDescent="0.35">
@@ -28950,32 +28950,6 @@
         <f t="shared" si="95"/>
         <v>950</v>
       </c>
-      <c r="DX12" t="str">
-        <f t="shared" si="0"/>
-        <v>[11,6950,7000],</v>
-      </c>
-      <c r="DZ12">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="EA12">
-        <f t="shared" si="4"/>
-        <v>6950</v>
-      </c>
-      <c r="EB12">
-        <v>50</v>
-      </c>
-      <c r="EC12">
-        <v>11</v>
-      </c>
-      <c r="ED12">
-        <f t="shared" si="1"/>
-        <v>0.70541760722347635</v>
-      </c>
-      <c r="EE12">
-        <f t="shared" si="2"/>
-        <v>7.7595936794582396</v>
-      </c>
     </row>
     <row r="13" spans="1:135" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -29403,32 +29377,6 @@
         <f t="shared" si="95"/>
         <v>980</v>
       </c>
-      <c r="DX13" t="str">
-        <f t="shared" si="0"/>
-        <v>[12,7000,7025],</v>
-      </c>
-      <c r="DZ13">
-        <f t="shared" si="3"/>
-        <v>7025</v>
-      </c>
-      <c r="EA13">
-        <f t="shared" si="4"/>
-        <v>7000</v>
-      </c>
-      <c r="EB13">
-        <v>25</v>
-      </c>
-      <c r="EC13">
-        <v>12</v>
-      </c>
-      <c r="ED13">
-        <f t="shared" si="1"/>
-        <v>0.35270880361173818</v>
-      </c>
-      <c r="EE13">
-        <f t="shared" si="2"/>
-        <v>4.2325056433408577</v>
-      </c>
     </row>
     <row r="14" spans="1:135" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -29856,31 +29804,9 @@
         <f t="shared" si="95"/>
         <v>995</v>
       </c>
-      <c r="DX14" t="str">
-        <f t="shared" si="0"/>
-        <v>[13,7025,7045],</v>
-      </c>
-      <c r="DZ14">
-        <f t="shared" si="3"/>
-        <v>7045</v>
-      </c>
-      <c r="EA14">
-        <f t="shared" si="4"/>
-        <v>7025</v>
-      </c>
       <c r="EB14">
-        <v>20</v>
-      </c>
-      <c r="EC14">
-        <v>13</v>
-      </c>
-      <c r="ED14">
-        <f t="shared" si="1"/>
-        <v>0.28216704288939054</v>
-      </c>
-      <c r="EE14">
-        <f t="shared" si="2"/>
-        <v>3.668171557562077</v>
+        <f>SUM(EB1:EB13)</f>
+        <v>17975</v>
       </c>
     </row>
     <row r="15" spans="1:135" x14ac:dyDescent="0.35">
@@ -30309,32 +30235,6 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX15" t="str">
-        <f t="shared" si="0"/>
-        <v>[14,7045,7060],</v>
-      </c>
-      <c r="DZ15">
-        <f t="shared" si="3"/>
-        <v>7060</v>
-      </c>
-      <c r="EA15">
-        <f t="shared" si="4"/>
-        <v>7045</v>
-      </c>
-      <c r="EB15">
-        <v>15</v>
-      </c>
-      <c r="EC15">
-        <v>14</v>
-      </c>
-      <c r="ED15">
-        <f t="shared" si="1"/>
-        <v>0.21162528216704291</v>
-      </c>
-      <c r="EE15">
-        <f t="shared" si="2"/>
-        <v>2.9627539503386009</v>
-      </c>
     </row>
     <row r="16" spans="1:135" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -30762,34 +30662,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX16" t="str">
-        <f t="shared" si="0"/>
-        <v>[15,7060,7070],</v>
-      </c>
-      <c r="DZ16">
-        <f t="shared" si="3"/>
-        <v>7070</v>
-      </c>
-      <c r="EA16">
-        <f t="shared" si="4"/>
-        <v>7060</v>
-      </c>
-      <c r="EB16">
-        <v>10</v>
-      </c>
-      <c r="EC16">
-        <v>15</v>
-      </c>
-      <c r="ED16">
-        <f t="shared" si="1"/>
-        <v>0.14108352144469527</v>
-      </c>
-      <c r="EE16">
-        <f t="shared" si="2"/>
-        <v>2.1162528216704288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -31215,34 +31089,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX17" t="str">
-        <f t="shared" si="0"/>
-        <v>[16,7070,7077],</v>
-      </c>
-      <c r="DZ17">
-        <f t="shared" si="3"/>
-        <v>7077</v>
-      </c>
-      <c r="EA17">
-        <f t="shared" si="4"/>
-        <v>7070</v>
-      </c>
-      <c r="EB17">
-        <v>7</v>
-      </c>
-      <c r="EC17">
-        <v>16</v>
-      </c>
-      <c r="ED17">
-        <f t="shared" si="1"/>
-        <v>9.8758465011286684E-2</v>
-      </c>
-      <c r="EE17">
-        <f t="shared" si="2"/>
-        <v>1.5801354401805869</v>
-      </c>
-    </row>
-    <row r="18" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -31668,34 +31516,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX18" t="str">
-        <f t="shared" si="0"/>
-        <v>[17,7077,7082],</v>
-      </c>
-      <c r="DZ18">
-        <f t="shared" si="3"/>
-        <v>7082</v>
-      </c>
-      <c r="EA18">
-        <f t="shared" si="4"/>
-        <v>7077</v>
-      </c>
-      <c r="EB18">
-        <v>5</v>
-      </c>
-      <c r="EC18">
-        <v>17</v>
-      </c>
-      <c r="ED18">
-        <f t="shared" si="1"/>
-        <v>7.0541760722347635E-2</v>
-      </c>
-      <c r="EE18">
-        <f t="shared" si="2"/>
-        <v>1.1992099322799099</v>
-      </c>
-    </row>
-    <row r="19" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0</v>
       </c>
@@ -32121,34 +31943,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX19" t="str">
-        <f t="shared" si="0"/>
-        <v>[18,7082,7085],</v>
-      </c>
-      <c r="DZ19">
-        <f t="shared" si="3"/>
-        <v>7085</v>
-      </c>
-      <c r="EA19">
-        <f t="shared" si="4"/>
-        <v>7082</v>
-      </c>
-      <c r="EB19">
-        <v>3</v>
-      </c>
-      <c r="EC19">
-        <v>18</v>
-      </c>
-      <c r="ED19">
-        <f t="shared" si="1"/>
-        <v>4.232505643340858E-2</v>
-      </c>
-      <c r="EE19">
-        <f t="shared" si="2"/>
-        <v>0.76185101580135439</v>
-      </c>
-    </row>
-    <row r="20" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -32574,34 +32370,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX20" t="str">
-        <f t="shared" si="0"/>
-        <v>[19,7085,7087],</v>
-      </c>
-      <c r="DZ20">
-        <f t="shared" si="3"/>
-        <v>7087</v>
-      </c>
-      <c r="EA20">
-        <f t="shared" si="4"/>
-        <v>7085</v>
-      </c>
-      <c r="EB20">
-        <v>2</v>
-      </c>
-      <c r="EC20">
-        <v>19</v>
-      </c>
-      <c r="ED20">
-        <f t="shared" si="1"/>
-        <v>2.8216704288939048E-2</v>
-      </c>
-      <c r="EE20">
-        <f t="shared" si="2"/>
-        <v>0.53611738148984189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -33027,34 +32797,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="DX21" t="str">
-        <f t="shared" si="0"/>
-        <v>[20,7087,7088],</v>
-      </c>
-      <c r="DZ21">
-        <f t="shared" si="3"/>
-        <v>7088</v>
-      </c>
-      <c r="EA21">
-        <f t="shared" si="4"/>
-        <v>7087</v>
-      </c>
-      <c r="EB21">
-        <v>1</v>
-      </c>
-      <c r="EC21">
-        <v>20</v>
-      </c>
-      <c r="ED21">
-        <f t="shared" si="1"/>
-        <v>1.4108352144469524E-2</v>
-      </c>
-      <c r="EE21">
-        <f t="shared" si="2"/>
-        <v>0.28216704288939048</v>
-      </c>
-    </row>
-    <row r="22" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -33481,7 +33225,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -33907,16 +33651,8 @@
         <f t="shared" si="95"/>
         <v>1000</v>
       </c>
-      <c r="EB23">
-        <f>SUM(EB1:EB22)</f>
-        <v>7088</v>
-      </c>
-      <c r="EE23">
-        <f>SUM(EE1:EE22)/100</f>
-        <v>4.0073363431151252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:135" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -34343,7 +34079,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -34770,7 +34506,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0</v>
       </c>
@@ -35059,7 +34795,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0</v>
       </c>
@@ -35072,7 +34808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0</v>
       </c>
@@ -35085,7 +34821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0</v>
       </c>
@@ -35190,7 +34926,7 @@
         <v>[1,50,115,0,1000]</v>
       </c>
     </row>
-    <row r="30" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>-1</v>
       </c>
@@ -35295,7 +35031,7 @@
         <v>[2,115,190,0,1000]</v>
       </c>
     </row>
-    <row r="31" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0</v>
       </c>
@@ -35400,7 +35136,7 @@
         <v>[3,190,290,0,1000]</v>
       </c>
     </row>
-    <row r="32" spans="1:135" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0</v>
       </c>

</xml_diff>